<commit_message>
Add control for number of parallel instances.
</commit_message>
<xml_diff>
--- a/Tests/Runner.xlsx
+++ b/Tests/Runner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishna.teja.taduri\PycharmProjects\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD6DBD8-E4CB-43AA-8F4A-8A77F349D635}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA3E25B-25E8-4D30-AD3E-E6452B3FADF6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{C4BE3A58-1781-4E19-BD1B-5C09003FE51D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C4BE3A58-1781-4E19-BD1B-5C09003FE51D}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="45">
   <si>
     <t>ExecutionFlag</t>
   </si>
@@ -78,12 +78,6 @@
   </si>
   <si>
     <t>Parallel</t>
-  </si>
-  <si>
-    <t>Instances</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>ST</t>
@@ -242,11 +236,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7044,10 +7037,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2946EC-E5BC-406D-AFBA-59B9538A1B98}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7056,7 +7049,7 @@
     <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -7067,26 +7060,20 @@
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
+      <c r="C2" s="2">
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -7108,8 +7095,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7123,25 +7110,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -7153,19 +7140,19 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -7176,10 +7163,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>5</v>
@@ -7188,7 +7175,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -7199,19 +7186,19 @@
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -7222,10 +7209,10 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>5</v>
@@ -7234,7 +7221,7 @@
         <v>6</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -7245,33 +7232,33 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
@@ -7280,7 +7267,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -7291,16 +7278,16 @@
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -7312,19 +7299,19 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -7335,10 +7322,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>5</v>
@@ -7347,7 +7334,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -7358,19 +7345,19 @@
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -7444,21 +7431,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -7475,7 +7462,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -7492,7 +7479,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -7534,21 +7521,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -7565,7 +7552,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -7582,7 +7569,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -7629,18 +7616,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>35</v>
@@ -7654,7 +7641,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -7668,7 +7655,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>6</v>

</xml_diff>